<commit_message>
Update CPIExcel.xlsx with new package entry
</commit_message>
<xml_diff>
--- a/CPIExcel.xlsx
+++ b/CPIExcel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bharti.pal\Downloads\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Package Name</t>
   </si>
@@ -72,12 +72,22 @@
   </si>
   <si>
     <t>IFLOW</t>
+  </si>
+  <si>
+    <t>GZIP</t>
+  </si>
+  <si>
+    <t>IFlow</t>
+  </si>
+  <si>
+    <t>2025-08-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D912091-F28B-419E-969A-749E76A8C8AF}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -458,43 +468,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="25.26953125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F2" s="1">
@@ -502,23 +512,43 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>11</v>
       </c>
       <c r="F3" s="1">
         <v>45876</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>